<commit_message>
number of training examples
</commit_message>
<xml_diff>
--- a/train_data_clean.xlsx
+++ b/train_data_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365-my.sharepoint.com/personal/jamesedwin_mcghee_students_fhnw_ch/Documents/2022-09 - Research Methods/Project/Prototype/RMIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_0AE955A58790D4F22CAA02D04B5ED87656C5D82E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84A139A5-048B-485C-986A-B725CCC311ED}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_0AE955A58790D4F22CAA02D04B5ED87656C5D82E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4295C07-1467-4D55-83E4-D93B88EC0E00}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4545,7 +4545,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -4601,7 +4601,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4617,6 +4617,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4908,7 +4912,7 @@
   <dimension ref="A1:AQ327"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1"/>
+      <selection activeCell="V76" sqref="V76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5039,7 +5043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -5129,7 +5133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5219,7 +5223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5309,7 +5313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5405,7 +5409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5498,7 +5502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5588,7 +5592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5678,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5768,7 +5772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5858,7 +5862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5948,7 +5952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6041,7 +6045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6134,7 +6138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -6224,7 +6228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -6317,7 +6321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6407,7 +6411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6497,7 +6501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6590,7 +6594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6680,7 +6684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -6770,7 +6774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -6860,7 +6864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6950,7 +6954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -7043,7 +7047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -7133,7 +7137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -7223,7 +7227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -7322,7 +7326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -8135,7 +8139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -8234,7 +8238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -8324,7 +8328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -8411,7 +8415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -8501,7 +8505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -8594,7 +8598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>42</v>
       </c>
@@ -8675,7 +8679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43</v>
       </c>
@@ -8762,7 +8766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45</v>
       </c>
@@ -8945,7 +8949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>48</v>
       </c>
@@ -9038,7 +9042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -9221,7 +9225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -9395,7 +9399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -9488,7 +9492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>54</v>
       </c>
@@ -9662,7 +9666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>56</v>
       </c>
@@ -10193,7 +10197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>67</v>
       </c>
@@ -10364,7 +10368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>70</v>
       </c>
@@ -10538,7 +10542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>72</v>
       </c>
@@ -10730,7 +10734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>0</v>
       </c>
@@ -10817,7 +10821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>1</v>
       </c>
@@ -10904,7 +10908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2</v>
       </c>
@@ -10997,7 +11001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>3</v>
       </c>
@@ -11084,7 +11088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>5</v>
       </c>
@@ -11171,7 +11175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>6</v>
       </c>
@@ -11360,7 +11364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>8</v>
       </c>
@@ -11447,7 +11451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>9</v>
       </c>
@@ -11918,7 +11922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>14</v>
       </c>
@@ -12002,7 +12006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>15</v>
       </c>
@@ -12086,7 +12090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>16</v>
       </c>
@@ -12170,7 +12174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>17</v>
       </c>
@@ -12254,7 +12258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>18</v>
       </c>
@@ -12341,7 +12345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>19</v>
       </c>
@@ -12425,7 +12429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>20</v>
       </c>
@@ -12512,7 +12516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>21</v>
       </c>
@@ -12689,7 +12693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>23</v>
       </c>
@@ -12866,7 +12870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>25</v>
       </c>
@@ -12953,7 +12957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>26</v>
       </c>
@@ -13037,7 +13041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>27</v>
       </c>
@@ -13400,7 +13404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>31</v>
       </c>
@@ -13484,7 +13488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>32</v>
       </c>
@@ -13574,7 +13578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>33</v>
       </c>
@@ -13658,7 +13662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>34</v>
       </c>
@@ -13742,7 +13746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>35</v>
       </c>
@@ -13829,7 +13833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>36</v>
       </c>
@@ -13916,7 +13920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>37</v>
       </c>
@@ -14006,7 +14010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>38</v>
       </c>
@@ -14183,7 +14187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>40</v>
       </c>
@@ -14369,7 +14373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>42</v>
       </c>
@@ -14456,7 +14460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43</v>
       </c>
@@ -14543,7 +14547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44</v>
       </c>
@@ -14630,7 +14634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>45</v>
       </c>
@@ -14717,7 +14721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>46</v>
       </c>
@@ -14801,7 +14805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>47</v>
       </c>
@@ -14885,7 +14889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>48</v>
       </c>
@@ -14969,7 +14973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>49</v>
       </c>
@@ -15053,7 +15057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>50</v>
       </c>
@@ -15230,7 +15234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>52</v>
       </c>
@@ -15401,7 +15405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>54</v>
       </c>
@@ -15488,7 +15492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>55</v>
       </c>
@@ -15572,7 +15576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>56</v>
       </c>
@@ -15659,7 +15663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>57</v>
       </c>
@@ -15743,7 +15747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>58</v>
       </c>
@@ -15827,7 +15831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>59</v>
       </c>
@@ -15911,7 +15915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>60</v>
       </c>
@@ -15995,7 +15999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>61</v>
       </c>
@@ -16079,7 +16083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>62</v>
       </c>
@@ -16166,7 +16170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>63</v>
       </c>
@@ -16253,7 +16257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>64</v>
       </c>
@@ -16340,7 +16344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>65</v>
       </c>
@@ -16430,7 +16434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>66</v>
       </c>
@@ -16520,7 +16524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>67</v>
       </c>
@@ -16610,7 +16614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>68</v>
       </c>
@@ -16697,7 +16701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>69</v>
       </c>
@@ -16880,7 +16884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>71</v>
       </c>
@@ -16964,7 +16968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>78</v>
       </c>
@@ -17045,7 +17049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>79</v>
       </c>
@@ -17126,7 +17130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>80</v>
       </c>
@@ -17210,7 +17214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>81</v>
       </c>
@@ -17297,7 +17301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>82</v>
       </c>
@@ -17378,7 +17382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>84</v>
       </c>
@@ -17540,7 +17544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>87</v>
       </c>
@@ -17864,7 +17868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>93</v>
       </c>
@@ -18551,7 +18555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2</v>
       </c>
@@ -18638,7 +18642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>3</v>
       </c>
@@ -18722,7 +18726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>4</v>
       </c>
@@ -18818,7 +18822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>5</v>
       </c>
@@ -18902,7 +18906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>6</v>
       </c>
@@ -18986,7 +18990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>7</v>
       </c>
@@ -19070,7 +19074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>8</v>
       </c>
@@ -19154,7 +19158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>9</v>
       </c>
@@ -19244,7 +19248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>10</v>
       </c>
@@ -19331,7 +19335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>11</v>
       </c>
@@ -19418,7 +19422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>12</v>
       </c>
@@ -19505,7 +19509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>13</v>
       </c>
@@ -19592,7 +19596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>14</v>
       </c>
@@ -19679,7 +19683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>15</v>
       </c>
@@ -19766,7 +19770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>16</v>
       </c>
@@ -19850,7 +19854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>17</v>
       </c>
@@ -19934,7 +19938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>18</v>
       </c>
@@ -20018,7 +20022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>19</v>
       </c>
@@ -20102,7 +20106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>20</v>
       </c>
@@ -20186,7 +20190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>21</v>
       </c>
@@ -20270,7 +20274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>22</v>
       </c>
@@ -20357,7 +20361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>23</v>
       </c>
@@ -20444,7 +20448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>24</v>
       </c>
@@ -20528,7 +20532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>25</v>
       </c>
@@ -20612,7 +20616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>26</v>
       </c>
@@ -20696,7 +20700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>27</v>
       </c>
@@ -20786,7 +20790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>28</v>
       </c>
@@ -20879,7 +20883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>29</v>
       </c>
@@ -20966,7 +20970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>30</v>
       </c>
@@ -21053,7 +21057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>31</v>
       </c>
@@ -21137,7 +21141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>32</v>
       </c>
@@ -21221,7 +21225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>33</v>
       </c>
@@ -21305,7 +21309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>34</v>
       </c>
@@ -21389,7 +21393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>35</v>
       </c>
@@ -21473,7 +21477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>36</v>
       </c>
@@ -21557,7 +21561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>37</v>
       </c>
@@ -21641,7 +21645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>38</v>
       </c>
@@ -21725,7 +21729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>39</v>
       </c>
@@ -21809,7 +21813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>40</v>
       </c>
@@ -21893,7 +21897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>41</v>
       </c>
@@ -21977,7 +21981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>42</v>
       </c>
@@ -22061,7 +22065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>43</v>
       </c>
@@ -22145,7 +22149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44</v>
       </c>
@@ -22232,7 +22236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>45</v>
       </c>
@@ -22319,7 +22323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>46</v>
       </c>
@@ -22403,7 +22407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>47</v>
       </c>
@@ -22490,7 +22494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>48</v>
       </c>
@@ -22583,7 +22587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>49</v>
       </c>
@@ -22670,7 +22674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>50</v>
       </c>
@@ -22760,7 +22764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>51</v>
       </c>
@@ -22847,7 +22851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>52</v>
       </c>
@@ -22931,7 +22935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>53</v>
       </c>
@@ -23018,7 +23022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>54</v>
       </c>
@@ -23102,7 +23106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>55</v>
       </c>
@@ -23189,7 +23193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>56</v>
       </c>
@@ -23273,7 +23277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>57</v>
       </c>
@@ -23366,7 +23370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>58</v>
       </c>
@@ -23456,7 +23460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>59</v>
       </c>
@@ -23540,7 +23544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>60</v>
       </c>
@@ -23633,7 +23637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>64</v>
       </c>
@@ -23810,7 +23814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>66</v>
       </c>
@@ -23894,7 +23898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>67</v>
       </c>
@@ -23981,7 +23985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>68</v>
       </c>
@@ -24065,7 +24069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>69</v>
       </c>
@@ -24254,7 +24258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>71</v>
       </c>
@@ -24344,7 +24348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>72</v>
       </c>
@@ -24437,7 +24441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>73</v>
       </c>
@@ -24527,7 +24531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>74</v>
       </c>
@@ -24617,7 +24621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>75</v>
       </c>
@@ -24698,7 +24702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>77</v>
       </c>
@@ -24782,7 +24786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>78</v>
       </c>
@@ -24956,7 +24960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>80</v>
       </c>
@@ -25622,7 +25626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>91</v>
       </c>
@@ -25718,7 +25722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>94</v>
       </c>
@@ -25808,7 +25812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>95</v>
       </c>
@@ -25895,7 +25899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>96</v>
       </c>
@@ -26081,7 +26085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>9</v>
       </c>
@@ -26168,7 +26172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>10</v>
       </c>
@@ -26255,7 +26259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>11</v>
       </c>
@@ -26342,7 +26346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>12</v>
       </c>
@@ -26429,7 +26433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>13</v>
       </c>
@@ -26516,7 +26520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>14</v>
       </c>
@@ -26603,7 +26607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>15</v>
       </c>
@@ -26690,7 +26694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>16</v>
       </c>
@@ -26780,7 +26784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>17</v>
       </c>
@@ -26867,7 +26871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>18</v>
       </c>
@@ -26954,7 +26958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>20</v>
       </c>
@@ -27041,7 +27045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>21</v>
       </c>
@@ -27125,7 +27129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>22</v>
       </c>
@@ -27209,7 +27213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>23</v>
       </c>
@@ -27293,7 +27297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>24</v>
       </c>
@@ -27380,7 +27384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>25</v>
       </c>
@@ -27467,7 +27471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>26</v>
       </c>
@@ -27551,7 +27555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>27</v>
       </c>
@@ -27638,7 +27642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>28</v>
       </c>
@@ -27725,7 +27729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>29</v>
       </c>
@@ -27812,7 +27816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>30</v>
       </c>
@@ -27902,7 +27906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>31</v>
       </c>
@@ -27989,7 +27993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>32</v>
       </c>
@@ -28076,7 +28080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>33</v>
       </c>
@@ -28163,7 +28167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>34</v>
       </c>
@@ -28250,7 +28254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>35</v>
       </c>
@@ -28337,7 +28341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>36</v>
       </c>
@@ -28424,7 +28428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>37</v>
       </c>
@@ -28511,7 +28515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>38</v>
       </c>
@@ -28601,7 +28605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>39</v>
       </c>
@@ -28691,7 +28695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>40</v>
       </c>
@@ -28781,7 +28785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>41</v>
       </c>
@@ -28871,7 +28875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>42</v>
       </c>
@@ -28964,7 +28968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>43</v>
       </c>
@@ -30458,7 +30462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>70</v>
       </c>
@@ -30797,7 +30801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>76</v>
       </c>
@@ -30965,7 +30969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>82</v>
       </c>
@@ -31136,7 +31140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>84</v>
       </c>
@@ -31226,7 +31230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>87</v>
       </c>
@@ -31388,7 +31392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>89</v>
       </c>
@@ -31481,7 +31485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>90</v>
       </c>
@@ -31658,7 +31662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>92</v>
       </c>
@@ -31739,7 +31743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>93</v>
       </c>
@@ -31913,7 +31917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>97</v>
       </c>
@@ -32090,7 +32094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>99</v>
       </c>
@@ -32186,7 +32190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>100</v>
       </c>
@@ -32807,7 +32811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>108</v>
       </c>
@@ -32891,7 +32895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>109</v>
       </c>
@@ -32972,7 +32976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A321" s="1">
         <v>111</v>
       </c>
@@ -33050,7 +33054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A322" s="1">
         <v>112</v>
       </c>
@@ -33131,7 +33135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A323" s="1">
         <v>114</v>
       </c>
@@ -33296,7 +33300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A325" s="1">
         <v>117</v>
       </c>
@@ -33380,7 +33384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A326" s="1">
         <v>118</v>
       </c>
@@ -33551,11 +33555,6 @@
         <filter val="1"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="23">
-      <filters>
-        <filter val="accepted under condition informed"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
convert raw data to scaled
</commit_message>
<xml_diff>
--- a/train_data_clean.xlsx
+++ b/train_data_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fhnw365-my.sharepoint.com/personal/jamesedwin_mcghee_students_fhnw_ch/Documents/2022-09 - Research Methods/Project/Prototype/RMIS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_0AE955A58790D4F22CAA02D04B5ED87656C5D82E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4295C07-1467-4D55-83E4-D93B88EC0E00}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="11_0AE955A58790D4F22CAA02D04B5ED87656C5D82E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{874EF98B-2801-447F-835F-997B10C3A03C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4908,11 +4908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ327"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="V76" sqref="V76"/>
+    <sheetView tabSelected="1" topLeftCell="G310" workbookViewId="0">
+      <selection activeCell="Q287" sqref="Q287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7419,7 +7418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -7509,7 +7508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -7599,7 +7598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -7689,7 +7688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -7779,7 +7778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -7869,7 +7868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -7959,7 +7958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -8049,7 +8048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -8856,7 +8855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>47</v>
       </c>
@@ -9132,7 +9131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -9312,7 +9311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -9573,7 +9572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>55</v>
       </c>
@@ -9753,7 +9752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>57</v>
       </c>
@@ -9852,7 +9851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>58</v>
       </c>
@@ -9942,7 +9941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>61</v>
       </c>
@@ -10029,7 +10028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>62</v>
       </c>
@@ -10107,7 +10106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>64</v>
       </c>
@@ -10284,7 +10283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>69</v>
       </c>
@@ -10461,7 +10460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>71</v>
       </c>
@@ -10638,7 +10637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>73</v>
       </c>
@@ -15321,7 +15320,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>53</v>
       </c>
@@ -17463,7 +17462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>85</v>
       </c>
@@ -17628,7 +17627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>89</v>
       </c>
@@ -17703,7 +17702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>90</v>
       </c>
@@ -17781,7 +17780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>91</v>
       </c>
@@ -17961,7 +17960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>94</v>
       </c>
@@ -18033,7 +18032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>95</v>
       </c>
@@ -18126,7 +18125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>96</v>
       </c>
@@ -18204,7 +18203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>101</v>
       </c>
@@ -18294,7 +18293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>104</v>
       </c>
@@ -18378,7 +18377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>105</v>
       </c>
@@ -23724,7 +23723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>65</v>
       </c>
@@ -24162,7 +24161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>70</v>
       </c>
@@ -24867,7 +24866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>79</v>
       </c>
@@ -25044,7 +25043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>81</v>
       </c>
@@ -25128,7 +25127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>82</v>
       </c>
@@ -25218,7 +25217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>83</v>
       </c>
@@ -25296,7 +25295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>84</v>
       </c>
@@ -25377,7 +25376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>86</v>
       </c>
@@ -25464,7 +25463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>87</v>
       </c>
@@ -25551,7 +25550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>88</v>
       </c>
@@ -25989,7 +25988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>97</v>
       </c>
@@ -29799,7 +29798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>57</v>
       </c>
@@ -29889,7 +29888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>58</v>
       </c>
@@ -29976,7 +29975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>59</v>
       </c>
@@ -30066,7 +30065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>60</v>
       </c>
@@ -30147,7 +30146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>61</v>
       </c>
@@ -30219,7 +30218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>62</v>
       </c>
@@ -30303,7 +30302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>63</v>
       </c>
@@ -30381,7 +30380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>64</v>
       </c>
@@ -30552,7 +30551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>71</v>
       </c>
@@ -30630,7 +30629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>72</v>
       </c>
@@ -30711,7 +30710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>74</v>
       </c>
@@ -30885,7 +30884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>81</v>
       </c>
@@ -31059,7 +31058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>83</v>
       </c>
@@ -31314,7 +31313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>88</v>
       </c>
@@ -31578,7 +31577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>91</v>
       </c>
@@ -31836,7 +31835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>94</v>
       </c>
@@ -32001,7 +32000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>98</v>
       </c>
@@ -32277,7 +32276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>101</v>
       </c>
@@ -32373,7 +32372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>102</v>
       </c>
@@ -32466,7 +32465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>103</v>
       </c>
@@ -32562,7 +32561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>104</v>
       </c>
@@ -33216,7 +33215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:43" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A324" s="1">
         <v>115</v>
       </c>
@@ -33544,18 +33543,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AQ327" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="19">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="20">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AQ327" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>